<commit_message>
Alteração IM feita, aguardando ok carlos.
</commit_message>
<xml_diff>
--- a/outputs/autoaprop.xlsx/autoapropxlsx/IMC_APQI.XLSX
+++ b/outputs/autoaprop.xlsx/autoapropxlsx/IMC_APQI.XLSX
@@ -133,12 +133,6 @@
     <t>ROBERTO NAZARIO DA SILVA</t>
   </si>
   <si>
-    <t>GILSON PAULA FERREIRA</t>
-  </si>
-  <si>
-    <t>ADEMIR JOSE DE LIMA CAVALCANTI</t>
-  </si>
-  <si>
     <t>DENILSON ALVES CRUZ</t>
   </si>
   <si>
@@ -148,19 +142,25 @@
     <t> </t>
   </si>
   <si>
-    <t>80</t>
+    <t> </t>
   </si>
   <si>
-    <t>2128</t>
+    <t> </t>
   </si>
   <si>
-    <t>2466</t>
+    <t>80</t>
   </si>
   <si>
     <t>2550</t>
   </si>
   <si>
     <t>3030</t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t> </t>
   </si>
   <si>
     <t> </t>
@@ -3524,19 +3524,19 @@
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>H12</f>
-        <v>GILSON PAULA FERREIRA</v>
+        <v>DENILSON ALVES CRUZ</v>
       </c>
       <c r="P12" s="161" t="str">
         <f>I12</f>
-        <v>ADEMIR JOSE DE LIMA CAVALCANTI</v>
+        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
       </c>
       <c r="Q12" s="161" t="str">
         <f>J12</f>
-        <v>DENILSON ALVES CRUZ</v>
+        <v> </v>
       </c>
       <c r="R12" s="161" t="str">
         <f>K12</f>
-        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
+        <v> </v>
       </c>
       <c r="S12" s="161" t="str">
         <f>L12</f>
@@ -3551,19 +3551,19 @@
       <c r="W12" s="161"/>
       <c r="X12" s="161" t="str">
         <f>H12</f>
-        <v>GILSON PAULA FERREIRA</v>
+        <v>DENILSON ALVES CRUZ</v>
       </c>
       <c r="Y12" s="161" t="str">
         <f>I12</f>
-        <v>ADEMIR JOSE DE LIMA CAVALCANTI</v>
+        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
       </c>
       <c r="Z12" s="161" t="str">
         <f>J12</f>
-        <v>DENILSON ALVES CRUZ</v>
+        <v> </v>
       </c>
       <c r="AA12" s="161" t="str">
         <f>K12</f>
-        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
+        <v> </v>
       </c>
       <c r="AB12" s="161" t="str">
         <f>L12</f>
@@ -3575,19 +3575,19 @@
       </c>
       <c r="AD12" s="183" t="str">
         <f t="shared" si="0"/>
-        <v>GILSON PAULA FERREIRA</v>
+        <v>DENILSON ALVES CRUZ</v>
       </c>
       <c r="AE12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>ADEMIR JOSE DE LIMA CAVALCANTI</v>
+        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
       </c>
       <c r="AF12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>DENILSON ALVES CRUZ</v>
+        <v> </v>
       </c>
       <c r="AG12" s="161" t="str">
         <f t="shared" si="0"/>
-        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
+        <v> </v>
       </c>
       <c r="AH12" s="161" t="str">
         <f t="shared" si="0"/>
@@ -3599,19 +3599,19 @@
       </c>
       <c r="AJ12" s="183" t="str">
         <f t="shared" si="1"/>
-        <v>GILSON PAULA FERREIRA</v>
+        <v>DENILSON ALVES CRUZ</v>
       </c>
       <c r="AK12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>ADEMIR JOSE DE LIMA CAVALCANTI</v>
+        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
       </c>
       <c r="AL12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>DENILSON ALVES CRUZ</v>
+        <v> </v>
       </c>
       <c r="AM12" s="161" t="str">
         <f t="shared" si="1"/>
-        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
+        <v> </v>
       </c>
       <c r="AN12" s="161" t="str">
         <f t="shared" si="1"/>
@@ -3904,19 +3904,19 @@
       <c r="N19" s="172"/>
       <c r="O19" s="172" t="str">
         <f>H19</f>
-        <v>2128</v>
+        <v>2550</v>
       </c>
       <c r="P19" s="172" t="str">
         <f>I19</f>
-        <v>2466</v>
+        <v>3030</v>
       </c>
       <c r="Q19" s="172" t="str">
         <f>J19</f>
-        <v>2550</v>
+        <v> </v>
       </c>
       <c r="R19" s="172" t="str">
         <f>K19</f>
-        <v>3030</v>
+        <v> </v>
       </c>
       <c r="S19" s="172" t="str">
         <f>L19</f>
@@ -3931,19 +3931,19 @@
       <c r="W19" s="172"/>
       <c r="X19" s="172" t="str">
         <f>H19</f>
-        <v>2128</v>
+        <v>2550</v>
       </c>
       <c r="Y19" s="172" t="str">
         <f>I19</f>
-        <v>2466</v>
+        <v>3030</v>
       </c>
       <c r="Z19" s="172" t="str">
         <f>J19</f>
-        <v>2550</v>
+        <v> </v>
       </c>
       <c r="AA19" s="172" t="str">
         <f>K19</f>
-        <v>3030</v>
+        <v> </v>
       </c>
       <c r="AB19" s="172" t="str">
         <f>L19</f>
@@ -3955,19 +3955,19 @@
       </c>
       <c r="AD19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>2128</v>
+        <v>2550</v>
       </c>
       <c r="AE19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>2466</v>
+        <v>3030</v>
       </c>
       <c r="AF19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>2550</v>
+        <v> </v>
       </c>
       <c r="AG19" s="172" t="str">
         <f t="shared" si="2"/>
-        <v>3030</v>
+        <v> </v>
       </c>
       <c r="AH19" s="172" t="str">
         <f t="shared" si="2"/>
@@ -3979,19 +3979,19 @@
       </c>
       <c r="AJ19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>2128</v>
+        <v>2550</v>
       </c>
       <c r="AK19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>2466</v>
+        <v>3030</v>
       </c>
       <c r="AL19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>2550</v>
+        <v> </v>
       </c>
       <c r="AM19" s="172" t="str">
         <f t="shared" si="3"/>
-        <v>3030</v>
+        <v> </v>
       </c>
       <c r="AN19" s="172" t="str">
         <f t="shared" si="3"/>
@@ -6609,19 +6609,19 @@
       </c>
       <c r="H12" s="161" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v>GILSON PAULA FERREIRA</v>
+        <v>DENILSON ALVES CRUZ</v>
       </c>
       <c r="I12" s="161" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>ADEMIR JOSE DE LIMA CAVALCANTI</v>
+        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
       </c>
       <c r="J12" s="161" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
-        <v>DENILSON ALVES CRUZ</v>
+        <v> </v>
       </c>
       <c r="K12" s="161" t="str">
         <f>'Segunda a Sexta'!K12:K18</f>
-        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
+        <v> </v>
       </c>
       <c r="L12" s="161" t="str">
         <f>'Segunda a Sexta'!L12:L18</f>
@@ -6634,19 +6634,19 @@
       <c r="N12" s="161"/>
       <c r="O12" s="187" t="str">
         <f>'Segunda a Sexta'!H12:H18</f>
-        <v>GILSON PAULA FERREIRA</v>
+        <v>DENILSON ALVES CRUZ</v>
       </c>
       <c r="P12" s="187" t="str">
         <f>'Segunda a Sexta'!I12:I18</f>
-        <v>ADEMIR JOSE DE LIMA CAVALCANTI</v>
+        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
       </c>
       <c r="Q12" s="187" t="str">
         <f>'Segunda a Sexta'!J12:J18</f>
-        <v>DENILSON ALVES CRUZ</v>
+        <v> </v>
       </c>
       <c r="R12" s="187" t="str">
         <f>'Segunda a Sexta'!K12:K18</f>
-        <v>JOSE SERGIO DO NASCIMENTO SILVA</v>
+        <v> </v>
       </c>
       <c r="S12" s="161" t="str">
         <f>'Segunda a Sexta'!L12:L18</f>
@@ -6941,19 +6941,19 @@
       </c>
       <c r="H19" s="168" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v>2128</v>
+        <v>2550</v>
       </c>
       <c r="I19" s="168" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v>2466</v>
+        <v>3030</v>
       </c>
       <c r="J19" s="170" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
-        <v>2550</v>
+        <v> </v>
       </c>
       <c r="K19" s="172" t="str">
         <f>'Segunda a Sexta'!K19:K20</f>
-        <v>3030</v>
+        <v> </v>
       </c>
       <c r="L19" s="172" t="str">
         <f>'Segunda a Sexta'!L19:L20</f>
@@ -6966,19 +6966,19 @@
       <c r="N19" s="172"/>
       <c r="O19" s="257" t="str">
         <f>'Segunda a Sexta'!H19:H20</f>
-        <v>2128</v>
+        <v>2550</v>
       </c>
       <c r="P19" s="257" t="str">
         <f>'Segunda a Sexta'!I19:I20</f>
-        <v>2466</v>
+        <v>3030</v>
       </c>
       <c r="Q19" s="257" t="str">
         <f>'Segunda a Sexta'!J19:J20</f>
-        <v>2550</v>
+        <v> </v>
       </c>
       <c r="R19" s="257" t="str">
         <f>'Segunda a Sexta'!K19:K20</f>
-        <v>3030</v>
+        <v> </v>
       </c>
       <c r="S19" s="172" t="str">
         <f>'Segunda a Sexta'!L19:L20</f>

</xml_diff>